<commit_message>
Website [Add automation for edit KTP in KYC Verification and CSR, add item wait for element and wait for page load in several script
</commit_message>
<xml_diff>
--- a/Data Files/Website/DataFiles_CRM/DataExcel_KYCVideo/Data_CRM_NasabahBaru.xlsx
+++ b/Data Files/Website/DataFiles_CRM/DataExcel_KYCVideo/Data_CRM_NasabahBaru.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18320" windowHeight="6840"/>
+    <workbookView windowWidth="17930" windowHeight="6920"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -64,16 +64,16 @@
     <t>Test</t>
   </si>
   <si>
-    <t>11/10/2020</t>
-  </si>
-  <si>
-    <t>12/11/2020</t>
+    <t>06/11/2020</t>
+  </si>
+  <si>
+    <t>17/12/2020</t>
   </si>
   <si>
     <t>Semua</t>
   </si>
   <si>
-    <t>10110674@yopmail.com</t>
+    <t>10110813@yopmail.com</t>
   </si>
   <si>
     <t>Kantor</t>
@@ -97,10 +97,10 @@
     <t>Untuk regression</t>
   </si>
   <si>
-    <t>regression 12 November 2020</t>
-  </si>
-  <si>
-    <t>nasabah baru</t>
+    <t>regression 5 januari 2021</t>
+  </si>
+  <si>
+    <t>Tunaiku Leadgen</t>
   </si>
 </sst>
 </file>
@@ -108,12 +108,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,10 +136,72 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color rgb="FF5F6368"/>
-      <name val="Roboto"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -150,6 +212,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -158,35 +234,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -195,84 +257,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,19 +281,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,49 +425,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,109 +455,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,26 +475,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,6 +501,26 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -554,34 +559,23 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -599,144 +593,143 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -747,12 +740,12 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
@@ -1057,13 +1050,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="10.2727272727273" customWidth="1"/>
     <col min="2" max="2" width="16.3636363636364" customWidth="1"/>
@@ -1135,12 +1128,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2">
-        <v>10002703</v>
-      </c>
-      <c r="B2" s="6" t="s">
+        <v>10002903</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1182,37 +1175,24 @@
       <c r="P2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="4:14">
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2 K3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2">
+      <formula1>"RAJA WATI,KALIBATA,DUREN TIGA,CIKOKO,PENGADEGAN,PANCORAN,SLIPI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"ACEH,BALI,BANTEN,BENGKULU,DAISTA YOGYAKARTA,DKI JAKARTA,JAMBI,JAWA BARAT,JAWA TENGAH,JAWA TIMUR,GORONTALO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
       <formula1>"KAB. ADM. KEP. SERIBU,KOTA ADM. JAKARTA PUSAT,KOTA ADM. JAKARTA UTARA,KOTA ADM. JAKARTA BARAT,KOTA ADM. JAKARTA SELATAN,KOTA ADM. JAKARTA TIMUR"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2 J3">
-      <formula1>"ACEH,BALI,BANTEN,BENGKULU,DAISTA YOGYAKARTA,DKI JAKARTA,JAMBI,JAWA BARAT,JAWA TENGAH,JAWA TIMUR,GORONTALO"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2 L3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
       <formula1>"SETIA BUDI,TEBET,MAMPANG PRAPATAN,PASAR MINGGU,KEBAYORAN LAMA,CILANDAK,KEBAYORAN BARU,PANCORAN,JAGAKARSA,PESANGGRAHAN,PALMERAH"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 M3">
-      <formula1>"RAJA WATI,KALIBATA,DUREN TIGA,CIKOKO,PENGADEGAN,PANCORAN,SLIPI"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="10110674@yopmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="10110813@yopmail.com" tooltip="mailto:10110813@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Website update tc in test suite end to end
</commit_message>
<xml_diff>
--- a/Data Files/Website/DataFiles_CRM/DataExcel_KYCVideo/Data_CRM_NasabahBaru.xlsx
+++ b/Data Files/Website/DataFiles_CRM/DataExcel_KYCVideo/Data_CRM_NasabahBaru.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070"/>
+    <workbookView windowWidth="22368" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -108,10 +108,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -134,81 +134,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -217,6 +142,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -224,26 +209,57 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -255,24 +271,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,19 +287,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,49 +437,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,109 +467,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,8 +484,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,50 +501,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -578,151 +534,195 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1056,28 +1056,28 @@
   <sheetPr/>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="10.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="16.3636363636364" customWidth="1"/>
-    <col min="3" max="3" width="15.2727272727273" customWidth="1"/>
-    <col min="4" max="4" width="19.8181818181818" customWidth="1"/>
-    <col min="5" max="5" width="30.5454545454545" customWidth="1"/>
-    <col min="6" max="6" width="16.9090909090909" customWidth="1"/>
+    <col min="1" max="1" width="10.2685185185185" customWidth="1"/>
+    <col min="2" max="2" width="16.3611111111111" customWidth="1"/>
+    <col min="3" max="3" width="15.2685185185185" customWidth="1"/>
+    <col min="4" max="4" width="19.8148148148148" customWidth="1"/>
+    <col min="5" max="5" width="30.5462962962963" customWidth="1"/>
+    <col min="6" max="6" width="16.9074074074074" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="12.0909090909091" customWidth="1"/>
+    <col min="8" max="8" width="12.0925925925926" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="12.9090909090909" customWidth="1"/>
-    <col min="11" max="11" width="27.3636363636364" customWidth="1"/>
-    <col min="12" max="12" width="15.4545454545455" customWidth="1"/>
-    <col min="13" max="13" width="12.4545454545455" customWidth="1"/>
-    <col min="14" max="14" width="15.6363636363636" customWidth="1"/>
-    <col min="15" max="15" width="31.8181818181818" customWidth="1"/>
-    <col min="16" max="16" width="16.1818181818182" customWidth="1"/>
+    <col min="10" max="10" width="12.9074074074074" customWidth="1"/>
+    <col min="11" max="11" width="27.3611111111111" customWidth="1"/>
+    <col min="12" max="12" width="15.4537037037037" customWidth="1"/>
+    <col min="13" max="13" width="12.4537037037037" customWidth="1"/>
+    <col min="14" max="14" width="15.6388888888889" customWidth="1"/>
+    <col min="15" max="15" width="31.8148148148148" customWidth="1"/>
+    <col min="16" max="16" width="16.1851851851852" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">

</xml_diff>

<commit_message>
Update test suite end to end
</commit_message>
<xml_diff>
--- a/Data Files/Website/DataFiles_CRM/DataExcel_KYCVideo/Data_CRM_NasabahBaru.xlsx
+++ b/Data Files/Website/DataFiles_CRM/DataExcel_KYCVideo/Data_CRM_NasabahBaru.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>SearchKYC</t>
   </si>
@@ -64,7 +64,10 @@
     <t>Test</t>
   </si>
   <si>
-    <t>06/01/2021</t>
+    <t>01/01/2020</t>
+  </si>
+  <si>
+    <t>04/08/2021</t>
   </si>
   <si>
     <t>Semua</t>
@@ -94,10 +97,10 @@
     <t>SLIPI</t>
   </si>
   <si>
-    <t>Untuk regression</t>
-  </si>
-  <si>
-    <t>regression 2 February 2021</t>
+    <t>TESTING STAGING</t>
+  </si>
+  <si>
+    <t>REGRESSION</t>
   </si>
   <si>
     <t>Nasabah Baru</t>
@@ -108,10 +111,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -135,6 +138,74 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -142,33 +213,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -177,81 +233,6 @@
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -263,11 +244,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -287,187 +290,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,11 +484,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,17 +523,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,43 +581,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -590,139 +599,133 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -734,7 +737,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,7 +1059,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1075,7 +1077,7 @@
     <col min="11" max="11" width="27.3611111111111" customWidth="1"/>
     <col min="12" max="12" width="15.4537037037037" customWidth="1"/>
     <col min="13" max="13" width="12.4537037037037" customWidth="1"/>
-    <col min="14" max="14" width="15.6388888888889" customWidth="1"/>
+    <col min="14" max="14" width="20.3888888888889" customWidth="1"/>
     <col min="15" max="15" width="31.8148148148148" customWidth="1"/>
     <col min="16" max="16" width="16.1851851851852" customWidth="1"/>
   </cols>
@@ -1134,56 +1136,59 @@
       <c r="A2">
         <v>10003148</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
       <formula1>"ACEH,BALI,BANTEN,BENGKULU,DAISTA YOGYAKARTA,DKI JAKARTA,JAMBI,JAWA BARAT,JAWA TENGAH,JAWA TIMUR,GORONTALO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2">
+      <formula1>"RAJA WATI,KALIBATA,DUREN TIGA,CIKOKO,PENGADEGAN,PANCORAN,SLIPI"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
       <formula1>"KAB. ADM. KEP. SERIBU,KOTA ADM. JAKARTA PUSAT,KOTA ADM. JAKARTA UTARA,KOTA ADM. JAKARTA BARAT,KOTA ADM. JAKARTA SELATAN,KOTA ADM. JAKARTA TIMUR"</formula1>
@@ -1191,9 +1196,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
       <formula1>"SETIA BUDI,TEBET,MAMPANG PRAPATAN,PASAR MINGGU,KEBAYORAN LAMA,CILANDAK,KEBAYORAN BARU,PANCORAN,JAGAKARSA,PESANGGRAHAN,PALMERAH"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2">
-      <formula1>"RAJA WATI,KALIBATA,DUREN TIGA,CIKOKO,PENGADEGAN,PANCORAN,SLIPI"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>